<commit_message>
Forum Completed (Answer all + Post all ! )
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Toàn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Ngày</t>
   </si>
@@ -94,13 +95,109 @@
   </si>
   <si>
     <t>Slide + presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task tracker </t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assigned to </t>
+  </si>
+  <si>
+    <t>Toàn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm việc với 1 bảng trên csdl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">làm việc với 2 bảng trên ơ sở dữ liệu có ràng buộc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Câu hỏi: Nội dung câu hỏi có lựa chọn, có câu trả lời </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cập nhật thông tin 1 câu hỏi đấy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Framework structure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database interaction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push and take data in HTML - EJS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngôn ngữ cơ bản  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm bảng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lấy code lên </t>
+  </si>
+  <si>
+    <t>Làm 1 cái Forum (Câu trả lời)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Học đối tượng </t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thi thử </t>
+  </si>
+  <si>
+    <t>Từ vựng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng thể </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm đề </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiển thị đề </t>
+  </si>
+  <si>
+    <t>Forum</t>
+  </si>
+  <si>
+    <t>THêm từ (ND)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QL Từ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">QD thêm từ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">QL TỪ Admin </t>
+  </si>
+  <si>
+    <t>Hiển thị danh sách từ cần học theo thgian</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +205,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -177,11 +300,149 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -192,9 +453,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -206,6 +517,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,22 +889,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.875" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="79.25" style="3" customWidth="1"/>
+    <col min="3" max="3" width="74.375" style="3" customWidth="1"/>
     <col min="4" max="4" width="43.5" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="3"/>
+    <col min="5" max="5" width="18.75" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -549,368 +919,481 @@
       <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>3</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="23">
         <v>43518</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E2" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="23">
         <v>43525</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
         <v>5</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="23">
         <v>43532</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
         <v>6</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="23">
         <v>43539</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="E11" s="41"/>
+      <c r="F11" s="42"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
         <v>7</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="23">
         <v>43546</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
         <v>8</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="23">
         <v>43553</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="E17" s="41"/>
+      <c r="F17" s="42"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="42"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
         <v>9</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="23">
         <v>43560</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="E20" s="41"/>
+      <c r="F20" s="42"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="42"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
         <v>10</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="23">
         <v>43567</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="31" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="E23" s="41"/>
+      <c r="F23" s="42"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="42"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="42"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
         <v>11</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="23">
         <v>43574</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="E26" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="33"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="35"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="37"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
         <v>12</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="30">
         <v>43581</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="38" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="E29" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="44"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
         <v>13</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="23">
         <v>43588</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="31" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="E32" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="44"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="44"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="44"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="21">
         <v>14</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="23">
         <v>43595</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="E35" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="44"/>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="44"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="37"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
         <v>15</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="23">
         <v>43602</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="44"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
+  <mergeCells count="54">
+    <mergeCell ref="E2:E25"/>
+    <mergeCell ref="F2:F25"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A23:A25"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="A26:A28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="C26:C28"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
@@ -923,26 +1406,317 @@
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A23:A25"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="A20:A22"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D8:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="50.25" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="7" max="8" width="4.625" customWidth="1"/>
+    <col min="9" max="9" width="4.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="16">
+        <v>43595</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10">
+        <v>43581</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="11">
+        <v>43582</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="11">
+        <v>43584</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="11">
+        <v>43585</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="11">
+        <v>43586</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="11">
+        <v>43587</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="11">
+        <v>43589</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="12">
+        <v>43591</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="16">
+        <v>43602</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="10">
+        <v>43595</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="11">
+        <v>43596</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="11">
+        <v>43597</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="11">
+        <v>43598</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>